<commit_message>
updated measure time function and updated Time for Merge and quick sort
</commit_message>
<xml_diff>
--- a/Merge_sort_time.xlsx
+++ b/Merge_sort_time.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\FCAI\Second year\Semester 2\Data Structure\Assigments\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\FCAI\Second year\Semester 2\Data Structure\Assigments\Assignment 1\Program\Sorting-Algorithms-with-calculating-time-of-sorting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF894120-4E39-4116-9DA0-6F826EF3C22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA3C54C-73CD-4D75-BACC-8023CB705AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B0469072-155D-4BEC-B5D8-CBD3F515A47A}"/>
   </bookViews>
@@ -201,25 +201,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>118</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>339</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>496</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2937</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5694</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13535</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31277</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,25 +507,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>111</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>806</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2150</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6513</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32949</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2197,7 +2197,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2221,13 +2221,13 @@
         <v>200</v>
       </c>
       <c r="B2">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>200</v>
       </c>
       <c r="N2">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -2235,13 +2235,13 @@
         <v>500</v>
       </c>
       <c r="B3">
-        <v>339</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>500</v>
       </c>
       <c r="N3">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -2249,13 +2249,13 @@
         <v>1000</v>
       </c>
       <c r="B4">
-        <v>496</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>1000</v>
       </c>
       <c r="N4">
-        <v>111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -2263,13 +2263,13 @@
         <v>5000</v>
       </c>
       <c r="B5">
-        <v>2937</v>
+        <v>2</v>
       </c>
       <c r="M5">
         <v>5000</v>
       </c>
       <c r="N5">
-        <v>806</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -2277,13 +2277,13 @@
         <v>10000</v>
       </c>
       <c r="B6">
-        <v>5694</v>
+        <v>5</v>
       </c>
       <c r="M6">
         <v>10000</v>
       </c>
       <c r="N6">
-        <v>2150</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -2291,13 +2291,13 @@
         <v>20000</v>
       </c>
       <c r="B7">
-        <v>13535</v>
+        <v>10</v>
       </c>
       <c r="M7">
         <v>20000</v>
       </c>
       <c r="N7">
-        <v>6513</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -2305,13 +2305,13 @@
         <v>50000</v>
       </c>
       <c r="B8">
-        <v>31277</v>
+        <v>28</v>
       </c>
       <c r="M8">
         <v>50000</v>
       </c>
       <c r="N8">
-        <v>32949</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>